<commit_message>
PoS results with 40k German and new test in trio
</commit_message>
<xml_diff>
--- a/results/acl/mbert/results_pos.xlsx
+++ b/results/acl/mbert/results_pos.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aturt\Documents\typology_of_crosslingual\results\acl\mbert\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -19,55 +24,55 @@
     <t>Language</t>
   </si>
   <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Slovak</t>
+  </si>
+  <si>
+    <t>Norwegian</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>Indonesian</t>
+  </si>
+  <si>
+    <t>Finnish</t>
+  </si>
+  <si>
+    <t>Basque</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Turkish</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>Hebrew</t>
+  </si>
+  <si>
+    <t>Algerian</t>
+  </si>
+  <si>
+    <t>Maltese</t>
+  </si>
+  <si>
     <t>German</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>Slovak</t>
-  </si>
-  <si>
-    <t>Norwegian</t>
-  </si>
-  <si>
-    <t>Greek</t>
-  </si>
-  <si>
-    <t>Chinese</t>
-  </si>
-  <si>
-    <t>Vietnamese</t>
-  </si>
-  <si>
-    <t>Indonesian</t>
-  </si>
-  <si>
-    <t>Finnish</t>
-  </si>
-  <si>
-    <t>Basque</t>
-  </si>
-  <si>
-    <t>Korean</t>
-  </si>
-  <si>
-    <t>Turkish</t>
-  </si>
-  <si>
-    <t>Arabic</t>
-  </si>
-  <si>
-    <t>Hebrew</t>
-  </si>
-  <si>
-    <t>Algerian</t>
-  </si>
-  <si>
-    <t>Maltese</t>
-  </si>
-  <si>
-    <t>Japanese</t>
   </si>
   <si>
     <t>Thai</t>
@@ -79,8 +84,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,11 +148,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -189,7 +202,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,9 +234,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,6 +269,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,1131 +445,1133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
       <c r="B2">
-        <v>0.9037724523248835</v>
+        <v>0.89818534423050289</v>
       </c>
       <c r="C2">
-        <v>0.8397284942512814</v>
+        <v>0.83972849425128138</v>
       </c>
       <c r="D2">
-        <v>0.7610010620122823</v>
+        <v>0.76100106201228235</v>
       </c>
       <c r="E2">
-        <v>0.8408366809807453</v>
+        <v>0.84083668098074527</v>
       </c>
       <c r="F2">
-        <v>0.8144710717089163</v>
+        <v>0.81447107170891631</v>
       </c>
       <c r="G2">
-        <v>0.6014683474165397</v>
+        <v>0.60146834741653965</v>
       </c>
       <c r="H2">
         <v>0.5479983377199058</v>
       </c>
       <c r="I2">
-        <v>0.7337119637992335</v>
+        <v>0.73371196379923354</v>
       </c>
       <c r="J2">
-        <v>0.6829200720321374</v>
+        <v>0.68292007203213745</v>
       </c>
       <c r="K2">
-        <v>0.6089947822874822</v>
+        <v>0.60899478228748216</v>
       </c>
       <c r="L2">
-        <v>0.5997137184282219</v>
+        <v>0.59971371842822185</v>
       </c>
       <c r="M2">
+        <v>0.56314355635591262</v>
+      </c>
+      <c r="N2">
         <v>0.6265872466177218</v>
       </c>
-      <c r="N2">
-        <v>0.6205845684997923</v>
-      </c>
       <c r="O2">
-        <v>0.7214757353280694</v>
+        <v>0.62058456849979227</v>
       </c>
       <c r="P2">
-        <v>0.6420095119360946</v>
+        <v>0.72147573532806941</v>
       </c>
       <c r="Q2">
-        <v>0.4972987948469317</v>
+        <v>0.64200951193609457</v>
       </c>
       <c r="R2">
-        <v>0.5631435563559126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>0.49729879484693168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0.3868726844055237</v>
+        <v>0.83176153587066348</v>
       </c>
       <c r="C3">
-        <v>0.8981138430447962</v>
+        <v>0.89811384304479625</v>
       </c>
       <c r="D3">
         <v>0.7250757830919502</v>
       </c>
       <c r="E3">
-        <v>0.8488127315594476</v>
+        <v>0.84881273155944759</v>
       </c>
       <c r="F3">
-        <v>0.767009093971034</v>
+        <v>0.76700909397103401</v>
       </c>
       <c r="G3">
-        <v>0.5632788817783766</v>
+        <v>0.56327888177837659</v>
       </c>
       <c r="H3">
-        <v>0.5955708992926911</v>
+        <v>0.59557089929269114</v>
       </c>
       <c r="I3">
-        <v>0.7381694173122263</v>
+        <v>0.73816941731222629</v>
       </c>
       <c r="J3">
-        <v>0.60500168406871</v>
+        <v>0.60500168406871002</v>
       </c>
       <c r="K3">
-        <v>0.5506483664533512</v>
+        <v>0.55064836645335125</v>
       </c>
       <c r="L3">
-        <v>0.5133462445267767</v>
+        <v>0.51334624452677668</v>
       </c>
       <c r="M3">
-        <v>0.5505641630178512</v>
+        <v>0.53220781407881446</v>
       </c>
       <c r="N3">
-        <v>0.6405776355675311</v>
+        <v>0.55056416301785116</v>
       </c>
       <c r="O3">
-        <v>0.7221286628494442</v>
+        <v>0.64057763556753111</v>
       </c>
       <c r="P3">
-        <v>0.6647019198383294</v>
+        <v>0.72212866284944421</v>
       </c>
       <c r="Q3">
-        <v>0.5051364095655103</v>
+        <v>0.66470191983832938</v>
       </c>
       <c r="R3">
-        <v>0.5322078140788145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>0.50513640956551031</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.82929075836659505</v>
+      </c>
+      <c r="C4">
+        <v>0.88509364445809025</v>
+      </c>
+      <c r="D4">
+        <v>0.96568928461774639</v>
+      </c>
+      <c r="E4">
+        <v>0.85838194657660427</v>
+      </c>
+      <c r="F4">
+        <v>0.82714154129567086</v>
+      </c>
+      <c r="G4">
+        <v>0.64108074915566471</v>
+      </c>
+      <c r="H4">
+        <v>0.60078292907583664</v>
+      </c>
+      <c r="I4">
+        <v>0.77041756217377955</v>
+      </c>
+      <c r="J4">
+        <v>0.77655818237642005</v>
+      </c>
+      <c r="K4">
+        <v>0.72367209088117901</v>
+      </c>
+      <c r="L4">
+        <v>0.60600245624808102</v>
+      </c>
+      <c r="M4">
+        <v>0.62204482652747928</v>
+      </c>
+      <c r="N4">
+        <v>0.69473441817623582</v>
+      </c>
+      <c r="O4">
+        <v>0.74808105618667486</v>
+      </c>
+      <c r="P4">
+        <v>0.74577832361068463</v>
+      </c>
+      <c r="Q4">
+        <v>0.64246238870125882</v>
+      </c>
+      <c r="R4">
+        <v>0.67278170095179612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>0.7911421553576912</v>
-      </c>
-      <c r="C4">
-        <v>0.8850936444580902</v>
-      </c>
-      <c r="D4">
-        <v>0.9656892846177464</v>
-      </c>
-      <c r="E4">
-        <v>0.8583819465766043</v>
-      </c>
-      <c r="F4">
-        <v>0.8271415412956709</v>
-      </c>
-      <c r="G4">
-        <v>0.6410807491556647</v>
-      </c>
-      <c r="H4">
-        <v>0.6007829290758366</v>
-      </c>
-      <c r="I4">
-        <v>0.7704175621737795</v>
-      </c>
-      <c r="J4">
-        <v>0.77655818237642</v>
-      </c>
-      <c r="K4">
-        <v>0.723672090881179</v>
-      </c>
-      <c r="L4">
-        <v>0.606002456248081</v>
-      </c>
-      <c r="M4">
-        <v>0.6947344181762358</v>
-      </c>
-      <c r="N4">
-        <v>0.7480810561866749</v>
-      </c>
-      <c r="O4">
-        <v>0.7457783236106846</v>
-      </c>
-      <c r="P4">
-        <v>0.6424623887012588</v>
-      </c>
-      <c r="Q4">
-        <v>0.6727817009517961</v>
-      </c>
-      <c r="R4">
-        <v>0.6220448265274793</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
       <c r="B5">
-        <v>0.7692718414202763</v>
+        <v>0.87385703797637326</v>
       </c>
       <c r="C5">
-        <v>0.8544683975171862</v>
+        <v>0.85446839751718617</v>
       </c>
       <c r="D5">
-        <v>0.7756457318294067</v>
+        <v>0.77564573182940666</v>
       </c>
       <c r="E5">
         <v>0.9789094306881132</v>
       </c>
       <c r="F5">
-        <v>0.7917639991990923</v>
+        <v>0.79176399919909235</v>
       </c>
       <c r="G5">
-        <v>0.6221384235466862</v>
+        <v>0.62213842354668625</v>
       </c>
       <c r="H5">
-        <v>0.5662751117933658</v>
+        <v>0.56627511179336576</v>
       </c>
       <c r="I5">
         <v>0.8279049589534806</v>
       </c>
       <c r="J5">
-        <v>0.7456116932523527</v>
+        <v>0.74561169325235266</v>
       </c>
       <c r="K5">
-        <v>0.6140959754388307</v>
+        <v>0.61409597543883065</v>
       </c>
       <c r="L5">
-        <v>0.5691116598811987</v>
+        <v>0.56911165988119872</v>
       </c>
       <c r="M5">
-        <v>0.5960421811386237</v>
+        <v>0.5502903290395782</v>
       </c>
       <c r="N5">
-        <v>0.6836748314756724</v>
+        <v>0.59604218113862373</v>
       </c>
       <c r="O5">
-        <v>0.7661349529466729</v>
+        <v>0.68367483147567243</v>
       </c>
       <c r="P5">
-        <v>0.6691250083427885</v>
+        <v>0.76613495294667289</v>
       </c>
       <c r="Q5">
-        <v>0.5760194887539211</v>
+        <v>0.66912500834278854</v>
       </c>
       <c r="R5">
-        <v>0.5502903290395782</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+        <v>0.57601948875392106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.80445224459634213</v>
+      </c>
+      <c r="C6">
+        <v>0.77452429336781825</v>
+      </c>
+      <c r="D6">
+        <v>0.73766857565121002</v>
+      </c>
+      <c r="E6">
+        <v>0.75799002401625715</v>
+      </c>
+      <c r="F6">
+        <v>0.97579900240162576</v>
+      </c>
+      <c r="G6">
+        <v>0.52540181045630885</v>
+      </c>
+      <c r="H6">
+        <v>0.50471088121189733</v>
+      </c>
+      <c r="I6">
+        <v>0.67762793275447997</v>
+      </c>
+      <c r="J6">
+        <v>0.65915388878625536</v>
+      </c>
+      <c r="K6">
+        <v>0.57731387400702017</v>
+      </c>
+      <c r="L6">
+        <v>0.51902826528727142</v>
+      </c>
+      <c r="M6">
+        <v>0.55034176981341221</v>
+      </c>
+      <c r="N6">
+        <v>0.63024200997598379</v>
+      </c>
+      <c r="O6">
+        <v>0.60955108073157216</v>
+      </c>
+      <c r="P6">
+        <v>0.68317014594494729</v>
+      </c>
+      <c r="Q6">
+        <v>0.6662663957140218</v>
+      </c>
+      <c r="R6">
+        <v>0.61047478292998336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>0.7570663218178459</v>
-      </c>
-      <c r="C6">
-        <v>0.7745242933678183</v>
-      </c>
-      <c r="D6">
-        <v>0.73766857565121</v>
-      </c>
-      <c r="E6">
-        <v>0.7579900240162571</v>
-      </c>
-      <c r="F6">
-        <v>0.9757990024016258</v>
-      </c>
-      <c r="G6">
-        <v>0.5254018104563088</v>
-      </c>
-      <c r="H6">
-        <v>0.5047108812118973</v>
-      </c>
-      <c r="I6">
-        <v>0.67762793275448</v>
-      </c>
-      <c r="J6">
-        <v>0.6591538887862554</v>
-      </c>
-      <c r="K6">
-        <v>0.5773138740070202</v>
-      </c>
-      <c r="L6">
-        <v>0.5190282652872714</v>
-      </c>
-      <c r="M6">
-        <v>0.6302420099759838</v>
-      </c>
-      <c r="N6">
-        <v>0.6095510807315722</v>
-      </c>
-      <c r="O6">
-        <v>0.6831701459449473</v>
-      </c>
-      <c r="P6">
-        <v>0.6662663957140218</v>
-      </c>
-      <c r="Q6">
-        <v>0.6104747829299834</v>
-      </c>
-      <c r="R6">
-        <v>0.5503417698134122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
       <c r="B7">
-        <v>0.5101564324071912</v>
+        <v>0.48494046229278542</v>
       </c>
       <c r="C7">
-        <v>0.562456222274107</v>
+        <v>0.56245622227410697</v>
       </c>
       <c r="D7">
         <v>0.3678262899836563</v>
       </c>
       <c r="E7">
-        <v>0.6010273173009573</v>
+        <v>0.60102731730095726</v>
       </c>
       <c r="F7">
-        <v>0.5201494279710484</v>
+        <v>0.52014942797104835</v>
       </c>
       <c r="G7">
-        <v>0.9188419332243755</v>
+        <v>0.91884193322437546</v>
       </c>
       <c r="H7">
-        <v>0.5106700910576698</v>
+        <v>0.51067009105766981</v>
       </c>
       <c r="I7">
         <v>0.5731496614522531</v>
       </c>
       <c r="J7">
-        <v>0.5490077048797571</v>
+        <v>0.54900770487975714</v>
       </c>
       <c r="K7">
-        <v>0.5209432640672426</v>
+        <v>0.52094326406724256</v>
       </c>
       <c r="L7">
-        <v>0.4995563857109503</v>
+        <v>0.49955638571095029</v>
       </c>
       <c r="M7">
-        <v>0.4982488909642774</v>
+        <v>0.55998132150361901</v>
       </c>
       <c r="N7">
-        <v>0.4335279010039692</v>
+        <v>0.49824889096427738</v>
       </c>
       <c r="O7">
-        <v>0.5040859210833528</v>
+        <v>0.43352790100396921</v>
       </c>
       <c r="P7">
-        <v>0.4711650712117674</v>
+        <v>0.50408592108335282</v>
       </c>
       <c r="Q7">
-        <v>0.4247490077048798</v>
+        <v>0.47116507121176737</v>
       </c>
       <c r="R7">
-        <v>0.559981321503619</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+        <v>0.42474900770487978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>0.4412379757423672</v>
+        <v>0.54069427017984106</v>
       </c>
       <c r="C8">
-        <v>0.5872020075282308</v>
+        <v>0.58720200752823082</v>
       </c>
       <c r="D8">
-        <v>0.5648682559598495</v>
+        <v>0.56486825595984946</v>
       </c>
       <c r="E8">
-        <v>0.5613550815558344</v>
+        <v>0.56135508155583436</v>
       </c>
       <c r="F8">
-        <v>0.5371810957758261</v>
+        <v>0.53718109577582607</v>
       </c>
       <c r="G8">
-        <v>0.5622751986616479</v>
+        <v>0.56227519866164788</v>
       </c>
       <c r="H8">
-        <v>0.8945211208699289</v>
+        <v>0.89452112086992885</v>
       </c>
       <c r="I8">
-        <v>0.6282726892513593</v>
+        <v>0.62827268925135926</v>
       </c>
       <c r="J8">
         <v>0.550564617314931</v>
       </c>
       <c r="K8">
-        <v>0.5733166039314095</v>
+        <v>0.57331660393140949</v>
       </c>
       <c r="L8">
-        <v>0.5038895859473024</v>
+        <v>0.50388958594730238</v>
       </c>
       <c r="M8">
-        <v>0.5553324968632372</v>
+        <v>0.51693851944792979</v>
       </c>
       <c r="N8">
-        <v>0.5375993308239231</v>
+        <v>0.55533249686323716</v>
       </c>
       <c r="O8">
-        <v>0.5989125888749477</v>
+        <v>0.53759933082392308</v>
       </c>
       <c r="P8">
-        <v>0.551401087411125</v>
+        <v>0.59891258887494769</v>
       </c>
       <c r="Q8">
-        <v>0.4996235884567127</v>
+        <v>0.55140108741112503</v>
       </c>
       <c r="R8">
-        <v>0.5169385194479298</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>0.49962358845671268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9">
-        <v>0.3135471731923663</v>
+        <v>0.35167099722247108</v>
       </c>
       <c r="C9">
-        <v>0.4116566615894633</v>
+        <v>0.41165666158946329</v>
       </c>
       <c r="D9">
-        <v>0.444270226682197</v>
+        <v>0.44427022668219701</v>
       </c>
       <c r="E9">
-        <v>0.3193262252486336</v>
+        <v>0.31932622524863358</v>
       </c>
       <c r="F9">
-        <v>0.4361616342621629</v>
+        <v>0.43616163426216292</v>
       </c>
       <c r="G9">
-        <v>0.463981722067915</v>
+        <v>0.46398172206791499</v>
       </c>
       <c r="H9">
-        <v>0.5140220410357494</v>
+        <v>0.51402204103574944</v>
       </c>
       <c r="I9">
-        <v>0.557476928590628</v>
+        <v>0.55747692859062803</v>
       </c>
       <c r="J9">
-        <v>0.4663112624316818</v>
+        <v>0.46631126243168181</v>
       </c>
       <c r="K9">
-        <v>0.4727622972851895</v>
+        <v>0.47276229728518948</v>
       </c>
       <c r="L9">
-        <v>0.3951258847773497</v>
+        <v>0.39512588477734972</v>
       </c>
       <c r="M9">
-        <v>0.4454349968640803</v>
+        <v>0.43177134665352568</v>
       </c>
       <c r="N9">
-        <v>0.4371920078845982</v>
+        <v>0.44543499686408028</v>
       </c>
       <c r="O9">
-        <v>0.5891497177672251</v>
+        <v>0.43719200788459822</v>
       </c>
       <c r="P9">
-        <v>0.508601379804677</v>
+        <v>0.58914971776722513</v>
       </c>
       <c r="Q9">
-        <v>0.4043544485261177</v>
+        <v>0.50860137980467701</v>
       </c>
       <c r="R9">
-        <v>0.4317713466535257</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>0.40435444852611768</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10">
-        <v>0.2801408248311539</v>
+        <v>0.34825405949130622</v>
       </c>
       <c r="C10">
-        <v>0.4640034487713752</v>
+        <v>0.46400344877137523</v>
       </c>
       <c r="D10">
         <v>0.3678689466877425</v>
       </c>
       <c r="E10">
-        <v>0.3974709009915218</v>
+        <v>0.39747090099152182</v>
       </c>
       <c r="F10">
-        <v>0.4539445322603822</v>
+        <v>0.45394453226038223</v>
       </c>
       <c r="G10">
-        <v>0.7048426498060066</v>
+        <v>0.70484264980600664</v>
       </c>
       <c r="H10">
-        <v>0.4969104756430522</v>
+        <v>0.49691047564305219</v>
       </c>
       <c r="I10">
-        <v>0.5056761028883461</v>
+        <v>0.50567610288834608</v>
       </c>
       <c r="J10">
-        <v>0.4655841356516741</v>
+        <v>0.46558413565167411</v>
       </c>
       <c r="K10">
-        <v>0.4347607414858456</v>
+        <v>0.43476074148584559</v>
       </c>
       <c r="L10">
-        <v>0.4813191550510131</v>
+        <v>0.48131915505101308</v>
       </c>
       <c r="M10">
-        <v>0.450064664463285</v>
+        <v>0.48555826986636008</v>
       </c>
       <c r="N10">
-        <v>0.3494036499497054</v>
+        <v>0.45006466446328502</v>
       </c>
       <c r="O10">
-        <v>0.4863486133065096</v>
+        <v>0.34940364994970541</v>
       </c>
       <c r="P10">
-        <v>0.4605546773961776</v>
+        <v>0.48634861330650958</v>
       </c>
       <c r="Q10">
-        <v>0.4019974134214686</v>
+        <v>0.46055467739617761</v>
       </c>
       <c r="R10">
-        <v>0.4855582698663601</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
+        <v>0.40199741342146861</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>0.6544080604534005</v>
+        <v>0.7453400503778338</v>
       </c>
       <c r="C11">
-        <v>0.8025188916876574</v>
+        <v>0.80251889168765744</v>
       </c>
       <c r="D11">
-        <v>0.7477581863979849</v>
+        <v>0.74775818639798486</v>
       </c>
       <c r="E11">
-        <v>0.8038790931989924</v>
+        <v>0.80387909319899242</v>
       </c>
       <c r="F11">
-        <v>0.7140050377833753</v>
+        <v>0.71400503778337532</v>
       </c>
       <c r="G11">
-        <v>0.6330982367758187</v>
+        <v>0.63309823677581867</v>
       </c>
       <c r="H11">
-        <v>0.5950629722921914</v>
+        <v>0.59506297229219141</v>
       </c>
       <c r="I11">
-        <v>0.9049874055415618</v>
+        <v>0.90498740554156176</v>
       </c>
       <c r="J11">
         <v>0.7392443324937028</v>
       </c>
       <c r="K11">
-        <v>0.6463476070528967</v>
+        <v>0.64634760705289673</v>
       </c>
       <c r="L11">
-        <v>0.5987405541561713</v>
+        <v>0.59874055415617133</v>
       </c>
       <c r="M11">
-        <v>0.6411586901763224</v>
+        <v>0.57914357682619644</v>
       </c>
       <c r="N11">
+        <v>0.64115869017632243</v>
+      </c>
+      <c r="O11">
         <v>0.6859949622166247</v>
       </c>
-      <c r="O11">
-        <v>0.7662468513853904</v>
-      </c>
       <c r="P11">
-        <v>0.6704785894206549</v>
+        <v>0.76624685138539039</v>
       </c>
       <c r="Q11">
-        <v>0.5644836272040302</v>
+        <v>0.67047858942065486</v>
       </c>
       <c r="R11">
-        <v>0.5791435768261964</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v>0.56448362720403022</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>0.7355747961827719</v>
+        <v>0.78253175756809712</v>
       </c>
       <c r="C12">
-        <v>0.8485748593819125</v>
+        <v>0.84857485938191246</v>
       </c>
       <c r="D12">
-        <v>0.7685647475194337</v>
+        <v>0.76856474751943371</v>
       </c>
       <c r="E12">
-        <v>0.8394741831511091</v>
+        <v>0.83947418315110911</v>
       </c>
       <c r="F12">
-        <v>0.7858813120141566</v>
+        <v>0.78588131201415656</v>
       </c>
       <c r="G12">
-        <v>0.6468432029324401</v>
+        <v>0.64684320293244013</v>
       </c>
       <c r="H12">
-        <v>0.571193831763888</v>
+        <v>0.57119383176388805</v>
       </c>
       <c r="I12">
-        <v>0.7932756114516842</v>
+        <v>0.79327561145168424</v>
       </c>
       <c r="J12">
-        <v>0.9734563609934905</v>
+        <v>0.97345636099349053</v>
       </c>
       <c r="K12">
         <v>0.7702079251722177</v>
       </c>
       <c r="L12">
-        <v>0.6453896227011313</v>
+        <v>0.64538962270113132</v>
       </c>
       <c r="M12">
-        <v>0.7652151930733742</v>
+        <v>0.68002275169057702</v>
       </c>
       <c r="N12">
-        <v>0.6453896227011313</v>
+        <v>0.76521519307337416</v>
       </c>
       <c r="O12">
-        <v>0.7918852303608671</v>
+        <v>0.64538962270113132</v>
       </c>
       <c r="P12">
-        <v>0.6664349364848638</v>
+        <v>0.79188523036086711</v>
       </c>
       <c r="Q12">
-        <v>0.6364153447513113</v>
+        <v>0.66643493648486385</v>
       </c>
       <c r="R12">
-        <v>0.680022751690577</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>0.63641534475131134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>0.65651924181504884</v>
+      </c>
+      <c r="C13">
+        <v>0.66829408385985067</v>
+      </c>
+      <c r="D13">
+        <v>0.64499056371543451</v>
+      </c>
+      <c r="E13">
+        <v>0.64322638877492411</v>
+      </c>
+      <c r="F13">
+        <v>0.63276442110445552</v>
+      </c>
+      <c r="G13">
+        <v>0.57204398129154022</v>
+      </c>
+      <c r="H13">
+        <v>0.56076146713711328</v>
+      </c>
+      <c r="I13">
+        <v>0.69426438007713132</v>
+      </c>
+      <c r="J13">
+        <v>0.70554689423155825</v>
+      </c>
+      <c r="K13">
+        <v>0.94814146221383444</v>
+      </c>
+      <c r="L13">
+        <v>0.62755395093132027</v>
+      </c>
+      <c r="M13">
+        <v>0.69131041273488147</v>
+      </c>
+      <c r="N13">
+        <v>0.67764831377697543</v>
+      </c>
+      <c r="O13">
+        <v>0.58164437515385248</v>
+      </c>
+      <c r="P13">
+        <v>0.70345450069746451</v>
+      </c>
+      <c r="Q13">
+        <v>0.62816936079428898</v>
+      </c>
+      <c r="R13">
+        <v>0.58976778534503982</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
-        <v>0.5753261672273734</v>
-      </c>
-      <c r="C13">
-        <v>0.6682940838598507</v>
-      </c>
-      <c r="D13">
-        <v>0.6449905637154345</v>
-      </c>
-      <c r="E13">
-        <v>0.6432263887749241</v>
-      </c>
-      <c r="F13">
-        <v>0.6327644211044555</v>
-      </c>
-      <c r="G13">
-        <v>0.5720439812915402</v>
-      </c>
-      <c r="H13">
-        <v>0.5607614671371133</v>
-      </c>
-      <c r="I13">
-        <v>0.6942643800771313</v>
-      </c>
-      <c r="J13">
-        <v>0.7055468942315583</v>
-      </c>
-      <c r="K13">
-        <v>0.9481414622138344</v>
-      </c>
-      <c r="L13">
-        <v>0.6275539509313203</v>
-      </c>
-      <c r="M13">
-        <v>0.6776483137769754</v>
-      </c>
-      <c r="N13">
-        <v>0.5816443751538525</v>
-      </c>
-      <c r="O13">
-        <v>0.7034545006974645</v>
-      </c>
-      <c r="P13">
-        <v>0.628169360794289</v>
-      </c>
-      <c r="Q13">
-        <v>0.5897677853450398</v>
-      </c>
-      <c r="R13">
-        <v>0.6913104127348815</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>0.55041246562786439</v>
+      </c>
+      <c r="C14">
+        <v>0.56585348656842704</v>
+      </c>
+      <c r="D14">
+        <v>0.51632235775223856</v>
+      </c>
+      <c r="E14">
+        <v>0.55658182330959605</v>
+      </c>
+      <c r="F14">
+        <v>0.54991891701332585</v>
+      </c>
+      <c r="G14">
+        <v>0.467531551857858</v>
+      </c>
+      <c r="H14">
+        <v>0.48420644433476701</v>
+      </c>
+      <c r="I14">
+        <v>0.54353803849679194</v>
+      </c>
+      <c r="J14">
+        <v>0.57829796234929143</v>
+      </c>
+      <c r="K14">
+        <v>0.57149404216315303</v>
+      </c>
+      <c r="L14">
+        <v>0.95244306564196568</v>
+      </c>
+      <c r="M14">
+        <v>0.4936896284284002</v>
+      </c>
+      <c r="N14">
+        <v>0.55661707678206307</v>
+      </c>
+      <c r="O14">
+        <v>0.4608686455615878</v>
+      </c>
+      <c r="P14">
+        <v>0.56655855601776772</v>
+      </c>
+      <c r="Q14">
+        <v>0.48328985405062402</v>
+      </c>
+      <c r="R14">
+        <v>0.47824860748783748</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
-        <v>0.4917390255668114</v>
-      </c>
-      <c r="C14">
-        <v>0.6231307284129282</v>
-      </c>
-      <c r="D14">
-        <v>0.5524602026049205</v>
-      </c>
-      <c r="E14">
-        <v>0.6380849011095031</v>
-      </c>
-      <c r="F14">
-        <v>0.5460082006753497</v>
-      </c>
-      <c r="G14">
-        <v>0.5235166425470333</v>
-      </c>
-      <c r="H14">
-        <v>0.5393150024119633</v>
-      </c>
-      <c r="I14">
-        <v>0.6088398456343463</v>
-      </c>
-      <c r="J14">
-        <v>0.6566570188133141</v>
-      </c>
-      <c r="K14">
-        <v>0.6463458755426917</v>
-      </c>
-      <c r="L14">
-        <v>0.6449589966232513</v>
-      </c>
-      <c r="M14">
-        <v>0.649662325132658</v>
-      </c>
-      <c r="N14">
-        <v>0.5065123010130246</v>
-      </c>
-      <c r="O14">
-        <v>0.6315123010130246</v>
-      </c>
-      <c r="P14">
-        <v>0.5438977327544622</v>
-      </c>
-      <c r="Q14">
-        <v>0.5078388808490111</v>
-      </c>
-      <c r="R14">
-        <v>0.5821273516642547</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
       <c r="B15">
-        <v>0.433257198487288</v>
+        <v>0.40232897742164969</v>
       </c>
       <c r="C15">
-        <v>0.5032762946044108</v>
+        <v>0.50327629460441081</v>
       </c>
       <c r="D15">
-        <v>0.3463885872617666</v>
+        <v>0.34638858726176658</v>
       </c>
       <c r="E15">
-        <v>0.4327704347174898</v>
+        <v>0.43277043471748983</v>
       </c>
       <c r="F15">
-        <v>0.3803497210469166</v>
+        <v>0.38034972104691661</v>
       </c>
       <c r="G15">
-        <v>0.5187029617703224</v>
+        <v>0.51870296177032238</v>
       </c>
       <c r="H15">
-        <v>0.4326581046167671</v>
+        <v>0.43265810461676713</v>
       </c>
       <c r="I15">
-        <v>0.4411577489047815</v>
+        <v>0.44115774890478149</v>
       </c>
       <c r="J15">
-        <v>0.4828696596397948</v>
+        <v>0.48286965963979478</v>
       </c>
       <c r="K15">
-        <v>0.5024899838993522</v>
+        <v>0.50248998389935218</v>
       </c>
       <c r="L15">
         <v>0.4829445463736099</v>
       </c>
       <c r="M15">
-        <v>0.5418804058860973</v>
+        <v>0.92754708503388628</v>
       </c>
       <c r="N15">
-        <v>0.3736099150035571</v>
+        <v>0.54188040588609732</v>
       </c>
       <c r="O15">
-        <v>0.4884112779421125</v>
+        <v>0.37360991500355711</v>
       </c>
       <c r="P15">
-        <v>0.4594675553225746</v>
+        <v>0.48841127794211248</v>
       </c>
       <c r="Q15">
-        <v>0.3671322125285505</v>
+        <v>0.45946755532257461</v>
       </c>
       <c r="R15">
-        <v>0.9275470850338863</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+        <v>0.36713221252855049</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
-        <v>0.589197656204676</v>
+        <v>0.60512970548078804</v>
       </c>
       <c r="C16">
-        <v>0.7072576434414342</v>
+        <v>0.655061439438268</v>
       </c>
       <c r="D16">
-        <v>0.6485467308696409</v>
+        <v>0.61507704310512967</v>
       </c>
       <c r="E16">
-        <v>0.7196727968904102</v>
+        <v>0.60903062219621606</v>
       </c>
       <c r="F16">
-        <v>0.6243545860648605</v>
+        <v>0.63029061829529942</v>
       </c>
       <c r="G16">
-        <v>0.547078958055346</v>
+        <v>0.62775502243027115</v>
       </c>
       <c r="H16">
-        <v>0.5173754133549922</v>
+        <v>0.62034328067095768</v>
       </c>
       <c r="I16">
-        <v>0.666183210535476</v>
+        <v>0.67154281256095183</v>
       </c>
       <c r="J16">
-        <v>0.700643963566746</v>
+        <v>0.69143748780963521</v>
       </c>
       <c r="K16">
-        <v>0.6725068167314497</v>
+        <v>0.6979715233079774</v>
       </c>
       <c r="L16">
-        <v>0.5679642629227823</v>
+        <v>0.5769455822118198</v>
       </c>
       <c r="M16">
-        <v>0.7464175900678772</v>
+        <v>0.63038814121318509</v>
       </c>
       <c r="N16">
-        <v>0.5831061089516737</v>
+        <v>0.94187634094012096</v>
       </c>
       <c r="O16">
-        <v>0.6449498172535824</v>
+        <v>0.54739613809245169</v>
       </c>
       <c r="P16">
-        <v>0.5970296455299646</v>
+        <v>0.66091281451141015</v>
       </c>
       <c r="Q16">
-        <v>0.5382607182224285</v>
+        <v>0.64033547883752684</v>
       </c>
       <c r="R16">
-        <v>0.630330103846377</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
+        <v>0.57860347181587668</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17">
-        <v>0.5561177774565081</v>
+        <v>0.62613573788546251</v>
       </c>
       <c r="C17">
-        <v>0.7682039419786998</v>
+        <v>0.65101872246696035</v>
       </c>
       <c r="D17">
-        <v>0.7688304178111898</v>
+        <v>0.66031112334801767</v>
       </c>
       <c r="E17">
-        <v>0.7799624114500506</v>
+        <v>0.65421943832599116</v>
       </c>
       <c r="F17">
-        <v>0.7143752108332129</v>
+        <v>0.66296117841409696</v>
       </c>
       <c r="G17">
-        <v>0.5774661462098212</v>
+        <v>0.46651294052863429</v>
       </c>
       <c r="H17">
-        <v>0.5954411835574189</v>
+        <v>0.54240088105726869</v>
       </c>
       <c r="I17">
-        <v>0.784588694520746</v>
+        <v>0.67173733480176212</v>
       </c>
       <c r="J17">
-        <v>0.6640161919907475</v>
+        <v>0.5567524779735683</v>
       </c>
       <c r="K17">
-        <v>0.6110548889210159</v>
+        <v>0.52997659691629961</v>
       </c>
       <c r="L17">
-        <v>0.5354922654329912</v>
+        <v>0.4578400330396476</v>
       </c>
       <c r="M17">
-        <v>0.5922124234976628</v>
+        <v>0.47405011013215859</v>
       </c>
       <c r="N17">
-        <v>0.7628066117295552</v>
+        <v>0.52281800660792954</v>
       </c>
       <c r="O17">
-        <v>0.7718182256276805</v>
+        <v>0.96782075991189431</v>
       </c>
       <c r="P17">
-        <v>0.7287841549804829</v>
+        <v>0.79549834801762109</v>
       </c>
       <c r="Q17">
-        <v>0.6237289769167751</v>
+        <v>0.61928689427312777</v>
       </c>
       <c r="R17">
-        <v>0.579201002361332</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
+        <v>0.51951404185022021</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18">
-        <v>0.5139063222567219</v>
+        <v>0.55929180154588098</v>
       </c>
       <c r="C18">
-        <v>0.6430600515293652</v>
+        <v>0.64306005152936518</v>
       </c>
       <c r="D18">
-        <v>0.5401995111316641</v>
+        <v>0.54019951113166409</v>
       </c>
       <c r="E18">
-        <v>0.5496465614058268</v>
+        <v>0.54964656140582679</v>
       </c>
       <c r="F18">
-        <v>0.5993922177445993</v>
+        <v>0.59939221774459928</v>
       </c>
       <c r="G18">
-        <v>0.4410385148972716</v>
+        <v>0.44103851489727158</v>
       </c>
       <c r="H18">
-        <v>0.469709982162912</v>
+        <v>0.46970998216291199</v>
       </c>
       <c r="I18">
-        <v>0.616898989231684</v>
+        <v>0.61689898923168396</v>
       </c>
       <c r="J18">
-        <v>0.4909823611019357</v>
+        <v>0.49098236110193572</v>
       </c>
       <c r="K18">
         <v>0.4625751469908172</v>
       </c>
       <c r="L18">
-        <v>0.4131598070951972</v>
+        <v>0.41315980709519717</v>
       </c>
       <c r="M18">
+        <v>0.45471361564378682</v>
+      </c>
+      <c r="N18">
         <v>0.4656140582678206</v>
       </c>
-      <c r="N18">
-        <v>0.6397568870978397</v>
-      </c>
       <c r="O18">
-        <v>0.9672986721278986</v>
+        <v>0.63975688709783973</v>
       </c>
       <c r="P18">
-        <v>0.5848582942458875</v>
+        <v>0.96729867212789855</v>
       </c>
       <c r="Q18">
-        <v>0.5290348153531083</v>
+        <v>0.58485829424588753</v>
       </c>
       <c r="R18">
-        <v>0.4547136156437868</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
+        <v>0.52903481535310826</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19">
-        <v>0.06714736367733214</v>
+        <v>0.21180712032447049</v>
       </c>
       <c r="C19">
-        <v>0.3433979269941415</v>
+        <v>0.34339792699414151</v>
       </c>
       <c r="D19">
-        <v>0.3249211356466877</v>
+        <v>0.32492113564668768</v>
       </c>
       <c r="E19">
-        <v>0.1825146462370437</v>
+        <v>0.18251464623704369</v>
       </c>
       <c r="F19">
         <v>0.2947273546642632</v>
       </c>
       <c r="G19">
-        <v>0.2609283461018477</v>
+        <v>0.26092834610184767</v>
       </c>
       <c r="H19">
-        <v>0.3258224425416855</v>
+        <v>0.32582244254168552</v>
       </c>
       <c r="I19">
-        <v>0.3668319062640829</v>
+        <v>0.36683190626408291</v>
       </c>
       <c r="J19">
-        <v>0.3091482649842272</v>
+        <v>0.30914826498422721</v>
       </c>
       <c r="K19">
-        <v>0.2690401081568274</v>
+        <v>0.26904010815682738</v>
       </c>
       <c r="L19">
-        <v>0.288418206399279</v>
+        <v>0.28841820639927901</v>
       </c>
       <c r="M19">
-        <v>0.281207751239297</v>
+        <v>0.2947273546642632</v>
       </c>
       <c r="N19">
-        <v>0.2893195132942767</v>
+        <v>0.28120775123929698</v>
       </c>
       <c r="O19">
-        <v>0.3560162235241099</v>
+        <v>0.28931951329427669</v>
       </c>
       <c r="P19">
+        <v>0.35601622352410989</v>
+      </c>
+      <c r="Q19">
         <v>0.821991888237945</v>
       </c>
-      <c r="Q19">
-        <v>0.3600721045515998</v>
-      </c>
       <c r="R19">
-        <v>0.2947273546642632</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
+        <v>0.36007210455159983</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20">
-        <v>0.12516933080466</v>
+        <v>0.1608416869863632</v>
       </c>
       <c r="C20">
-        <v>0.3312562087961708</v>
+        <v>0.33125620879617079</v>
       </c>
       <c r="D20">
-        <v>0.2509708299467173</v>
+        <v>0.25097082994671732</v>
       </c>
       <c r="E20">
-        <v>0.1302266775038382</v>
+        <v>0.13022667750383821</v>
       </c>
       <c r="F20">
-        <v>0.2629820283572654</v>
+        <v>0.26298202835726542</v>
       </c>
       <c r="G20">
-        <v>0.1911857671814323</v>
+        <v>0.19118576718143229</v>
       </c>
       <c r="H20">
-        <v>0.31987717872302</v>
+        <v>0.31987717872302002</v>
       </c>
       <c r="I20">
         <v>0.3283662963966405</v>
       </c>
       <c r="J20">
-        <v>0.3204190372979319</v>
+        <v>0.32041903729793192</v>
       </c>
       <c r="K20">
-        <v>0.3256570035220807</v>
+        <v>0.32565700352208071</v>
       </c>
       <c r="L20">
-        <v>0.3105752731870315</v>
+        <v>0.31057527318703149</v>
       </c>
       <c r="M20">
-        <v>0.287636593515759</v>
+        <v>0.30109274812607251</v>
       </c>
       <c r="N20">
-        <v>0.1903729793190644</v>
+        <v>0.28763659351575899</v>
       </c>
       <c r="O20">
-        <v>0.332972094283392</v>
+        <v>0.19037297931906441</v>
       </c>
       <c r="P20">
-        <v>0.3800234805382462</v>
+        <v>0.33297209428339197</v>
       </c>
       <c r="Q20">
-        <v>0.9293777657364761</v>
+        <v>0.38002348053824619</v>
       </c>
       <c r="R20">
-        <v>0.3010927481260725</v>
+        <v>0.92937776573647612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>